<commit_message>
Update comprehensive README with enhanced RAG architecture documentation and latest campaign results
- Enhanced project overview with RAG architecture emphasis
- Updated pipeline workflow with GPT-4o and DALL-E 3 HD integration
- Added detailed RAG processing explanation with vector database metrics
- Updated campaign results with real 2025 data and semantic search scores
- Comprehensive system performance metrics and API cost analysis
- Enhanced technical implementation details for production deployment
- Added latest generated ad examples with contextual news connections
- Updated repository structure reflecting organized folder hierarchy

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/URL_and_news_articles_examples_by_client.xlsx
+++ b/URL_and_news_articles_examples_by_client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fundamentalmedia-my.sharepoint.com/personal/geoff_smith_fundamentalmedia_com/Documents/Documents/Alphix/Team/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/engs2742/news_generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{5C8DB88A-D5BC-49B6-B8FD-197F9419DDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DE8A8F2-3806-4513-8087-0E2182A6E6EB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34DF25F-3804-D649-B847-0FCE173C538B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A84E3AC9-DCE5-4040-A31B-AE7A13E88DC1}"/>
+    <workbookView xWindow="480" yWindow="2120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A84E3AC9-DCE5-4040-A31B-AE7A13E88DC1}"/>
   </bookViews>
   <sheets>
     <sheet name="PIMCO" sheetId="1" r:id="rId1"/>
@@ -1948,24 +1948,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262B5CD1-B922-490E-BA94-5B1F8DB8DC8E}">
   <dimension ref="A2:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="98.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>93</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -2706,23 +2706,23 @@
   <dimension ref="A2:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="98.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="150.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="150.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>239</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>237</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>235</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>232</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>230</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>227</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>225</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>221</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>219</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>217</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>215</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>213</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>211</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>209</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>207</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>205</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>203</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>200</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>198</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>194</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>191</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>189</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>187</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>185</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>183</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>181</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>178</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>176</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>170</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>168</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>159</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>157</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>155</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>152</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>149</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>147</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>145</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>142</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>140</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>135</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>132</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>129</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -3462,24 +3462,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA629E9-E271-4866-AB33-D434EE0C7802}">
   <dimension ref="A2:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="104.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="104.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>346</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>344</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>342</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>340</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>338</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>336</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>334</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>332</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>330</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>328</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>326</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>324</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>322</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>320</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>318</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>316</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>314</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>312</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>310</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>308</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>306</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>304</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>302</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>300</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>297</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>295</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>293</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>291</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>289</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>287</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>285</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>283</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>281</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>279</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>276</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>274</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>272</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>270</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>268</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>266</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>264</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>262</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>260</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>257</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>254</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>251</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>249</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>247</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>245</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>242</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>127</v>
       </c>

</xml_diff>